<commit_message>
Squashing commits to fix git history for recent updates
</commit_message>
<xml_diff>
--- a/tests/data/indicator_test_output_MINI_2405313_mod_2.xlsx
+++ b/tests/data/indicator_test_output_MINI_2405313_mod_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pmanko/code/who_l3_smart_tools/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3837454-A4BF-9A4C-B283-21BC8F928F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9342D956-38CF-BA4C-B262-DE70B48ADB26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19780" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HIV.IND.19" sheetId="1" r:id="rId1"/>
@@ -106,9 +106,6 @@
     <t>EXCLUSION: Clients with an "HIV treatment outcome" IN 'Lost to follow up', 'Transferred out', 'Death (documented)' at the end of the reporting period</t>
   </si>
   <si>
-    <t>"HIV status"='HIV-positive'</t>
-  </si>
-  <si>
     <t>"On ART"=True at reporting period end date</t>
   </si>
   <si>
@@ -125,6 +122,9 @@
 For progress towards 2nd 95 target: *Estimated number of people living with HIV who know their status
 For this purpose of test data:
 COUNT of client with "HIV status"='HIV-positive'</t>
+  </si>
+  <si>
+    <t>"HIV status"='HIV-positive' at reporting period end</t>
   </si>
 </sst>
 </file>
@@ -1147,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView zoomScale="200" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1774,8 +1774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="I13" zoomScale="175" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1784,7 +1784,7 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35.5" bestFit="1" customWidth="1"/>
@@ -1812,25 +1812,25 @@
         <v>22</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
CQL templates, CQL measures, and CQL common concepts
</commit_message>
<xml_diff>
--- a/tests/data/indicator_test_output_MINI_2405313_mod_2.xlsx
+++ b/tests/data/indicator_test_output_MINI_2405313_mod_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pmanko/code/who_l3_smart_tools/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3837454-A4BF-9A4C-B283-21BC8F928F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9342D956-38CF-BA4C-B262-DE70B48ADB26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19780" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HIV.IND.19" sheetId="1" r:id="rId1"/>
@@ -106,9 +106,6 @@
     <t>EXCLUSION: Clients with an "HIV treatment outcome" IN 'Lost to follow up', 'Transferred out', 'Death (documented)' at the end of the reporting period</t>
   </si>
   <si>
-    <t>"HIV status"='HIV-positive'</t>
-  </si>
-  <si>
     <t>"On ART"=True at reporting period end date</t>
   </si>
   <si>
@@ -125,6 +122,9 @@
 For progress towards 2nd 95 target: *Estimated number of people living with HIV who know their status
 For this purpose of test data:
 COUNT of client with "HIV status"='HIV-positive'</t>
+  </si>
+  <si>
+    <t>"HIV status"='HIV-positive' at reporting period end</t>
   </si>
 </sst>
 </file>
@@ -1147,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView zoomScale="200" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1774,8 +1774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="I13" zoomScale="175" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1784,7 +1784,7 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35.5" bestFit="1" customWidth="1"/>
@@ -1812,25 +1812,25 @@
         <v>22</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>22</v>

</xml_diff>